<commit_message>
Dev #378: correct AI upload
</commit_message>
<xml_diff>
--- a/spec/fixtures/files/reduced_categories_table.xlsx
+++ b/spec/fixtures/files/reduced_categories_table.xlsx
@@ -14,7 +14,7 @@
     <sheet name="Attainment" sheetId="4" state="visible" r:id="rId5"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="true" localSheetId="3" name="_xlnm._FilterDatabase" vbProcedure="false">Attainment!$A$1:$Y$180</definedName>
+    <definedName function="false" hidden="true" localSheetId="3" name="_xlnm._FilterDatabase" vbProcedure="false">Attainment!$A$1:$Y$179</definedName>
     <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Demographics!$A$5:$AM$40</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
@@ -63,7 +63,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1553" uniqueCount="1407">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1551" uniqueCount="1405">
   <si>
     <t xml:space="preserve">Category (L0) == the standard extract</t>
   </si>
@@ -912,8 +912,7 @@
     <t xml:space="preserve">IDACIRank_ab[yy]</t>
   </si>
   <si>
-    <t xml:space="preserve">IDACI Rank (based on pupil postcode)
-</t>
+    <t xml:space="preserve">IDACI Rank (based on pupil postcode)</t>
   </si>
   <si>
     <t xml:space="preserve">IDACI_R_home</t>
@@ -2963,125 +2962,118 @@
     <t xml:space="preserve">KS2_VAINPUT</t>
   </si>
   <si>
-    <t xml:space="preserve">KS2 average point score VA calculation</t>
-  </si>
-  <si>
-    <t xml:space="preserve">KS2 average point score used as the output measure in the calculation of value added.
-N.B. Not populated in Unamended data outputs</t>
+    <t xml:space="preserve">Included in old CVA calculations</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pupil included in old CVA calculations</t>
+  </si>
+  <si>
+    <t xml:space="preserve">KS2_INCVA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Included in VA calculations</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pupil included in VA calculations</t>
+  </si>
+  <si>
+    <t xml:space="preserve">KS2_INKS12VA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">English and Maths VA score </t>
+  </si>
+  <si>
+    <t xml:space="preserve">English + Maths VA score (Actual-predicted)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">KS2_VAAPSSCORE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">English VA score</t>
+  </si>
+  <si>
+    <t xml:space="preserve">English VA score (Actual-predicted)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">KS2_VAENGSCORE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Maths VA score</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Maths VA score (Actual-predicted)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">KS2_VAMATSCORE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Writing TA VA score </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Writing TA VA score (actual - predicted)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">KS2_VAWRITTASCORE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Overall VA score</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Overall VA score (actual - predicted)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">KS2_VAOSCORE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Reading VA score </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Reading VA score (actual - predicted)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">KS2_VAREADSCORE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Standard deviation of pupils CVAPAPS score</t>
+  </si>
+  <si>
+    <t xml:space="preserve">KS3_SC_KS2STDEV</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Total KS3 point score VA calculation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Total KS3 point score as used in the valued added calculations.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">KS3_TOTPTS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">KS4 EBacc science VA score</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pupil EBacc Science VA score</t>
+  </si>
+  <si>
+    <t xml:space="preserve">KS4_SCIVASCR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">KS4_EBPTSSCI_PTQ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">KS4_EBPTSSCI_PTQ_EE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">KS2 average point score VA calculation </t>
+  </si>
+  <si>
+    <t xml:space="preserve">KS2 average point score used as the input measure in the calculation of value added.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">KS3_VAINPUT</t>
   </si>
   <si>
     <t xml:space="preserve">KS2_VAOUTPUT</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Included in old CVA calculations</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Pupil included in old CVA calculations</t>
-  </si>
-  <si>
-    <t xml:space="preserve">KS2_INCVA</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Included in VA calculations</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Pupil included in VA calculations</t>
-  </si>
-  <si>
-    <t xml:space="preserve">KS2_INKS12VA</t>
-  </si>
-  <si>
-    <t xml:space="preserve">English and Maths VA score </t>
-  </si>
-  <si>
-    <t xml:space="preserve">English + Maths VA score (Actual-predicted)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">KS2_VAAPSSCORE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">English VA score</t>
-  </si>
-  <si>
-    <t xml:space="preserve">English VA score (Actual-predicted)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">KS2_VAENGSCORE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Maths VA score</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Maths VA score (Actual-predicted)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">KS2_VAMATSCORE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Writing TA VA score </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Writing TA VA score (actual - predicted)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">KS2_VAWRITTASCORE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Overall VA score</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Overall VA score (actual - predicted)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">KS2_VAOSCORE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Reading VA score </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Reading VA score (actual - predicted)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">KS2_VAREADSCORE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Standard deviation of pupils CVAPAPS score</t>
-  </si>
-  <si>
-    <t xml:space="preserve">KS3_SC_KS2STDEV</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Total KS3 point score VA calculation</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Total KS3 point score as used in the valued added calculations.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">KS3_TOTPTS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">KS4 EBacc science VA score</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Pupil EBacc Science VA score</t>
-  </si>
-  <si>
-    <t xml:space="preserve">KS4_SCIVASCR</t>
-  </si>
-  <si>
-    <t xml:space="preserve">KS4_EBPTSSCI_PTQ</t>
-  </si>
-  <si>
-    <t xml:space="preserve">KS4_EBPTSSCI_PTQ_EE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">KS2 average point score VA calculation </t>
-  </si>
-  <si>
-    <t xml:space="preserve">KS2 average point score used as the input measure in the calculation of value added.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">KS3_VAINPUT</t>
   </si>
   <si>
     <t xml:space="preserve">KS3 average point score VA calculation </t>
@@ -5215,9 +5207,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>27360</xdr:colOff>
+      <xdr:colOff>27000</xdr:colOff>
       <xdr:row>44</xdr:row>
-      <xdr:rowOff>132480</xdr:rowOff>
+      <xdr:rowOff>132120</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -5231,7 +5223,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="22943160" y="8239320"/>
-          <a:ext cx="27360" cy="8280"/>
+          <a:ext cx="27000" cy="7920"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -5257,10 +5249,10 @@
   </sheetPr>
   <dimension ref="A1:AM1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="5" topLeftCell="A21" activePane="bottomLeft" state="frozen"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="55" zoomScaleNormal="55" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="0" ySplit="5" topLeftCell="A35" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="A57" activeCellId="0" sqref="A57"/>
+      <selection pane="bottomLeft" activeCell="I48" activeCellId="0" sqref="I48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -5270,7 +5262,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="12.66"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="15.66"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="14.66"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="55.17"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="52.86"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="33.83"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="11" style="0" width="18.66"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="25" min="20" style="0" width="18.85"/>
@@ -9227,10 +9219,10 @@
   </sheetPr>
   <dimension ref="A1:AM79"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="5" topLeftCell="A26" activePane="bottomLeft" state="frozen"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="55" zoomScaleNormal="55" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="0" ySplit="5" topLeftCell="A52" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="B7" activeCellId="0" sqref="B7"/>
+      <selection pane="bottomLeft" activeCell="I6" activeCellId="0" sqref="I6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -11384,8 +11376,8 @@
   </sheetPr>
   <dimension ref="A1:AD1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A30" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A37" activeCellId="0" sqref="A37"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A13" colorId="64" zoomScale="55" zoomScaleNormal="55" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="I50" activeCellId="0" sqref="I50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -14423,10 +14415,10 @@
   </sheetPr>
   <dimension ref="A1:AD1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="55" zoomScaleNormal="55" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="A33" activeCellId="0" sqref="A33"/>
+      <selection pane="bottomLeft" activeCell="A50" activeCellId="0" sqref="A50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -16745,10 +16737,10 @@
         <v>986</v>
       </c>
       <c r="J58" s="107" t="s">
+        <v>986</v>
+      </c>
+      <c r="K58" s="107" t="s">
         <v>987</v>
-      </c>
-      <c r="K58" s="107" t="s">
-        <v>988</v>
       </c>
       <c r="L58" s="107"/>
       <c r="M58" s="107"/>
@@ -16780,7 +16772,7 @@
       <c r="G59" s="107"/>
       <c r="H59" s="107"/>
       <c r="I59" s="107" t="s">
-        <v>989</v>
+        <v>988</v>
       </c>
       <c r="J59" s="107" t="s">
         <v>989</v>
@@ -16826,8 +16818,12 @@
       <c r="K60" s="107" t="s">
         <v>993</v>
       </c>
-      <c r="L60" s="107"/>
-      <c r="M60" s="107"/>
+      <c r="L60" s="107" t="s">
+        <v>994</v>
+      </c>
+      <c r="M60" s="107" t="s">
+        <v>995</v>
+      </c>
       <c r="N60" s="107"/>
       <c r="O60" s="107"/>
       <c r="P60" s="107"/>
@@ -16856,20 +16852,18 @@
       <c r="G61" s="107"/>
       <c r="H61" s="107"/>
       <c r="I61" s="107" t="s">
-        <v>994</v>
+        <v>996</v>
       </c>
       <c r="J61" s="107" t="s">
-        <v>995</v>
+        <v>997</v>
       </c>
       <c r="K61" s="107" t="s">
-        <v>996</v>
+        <v>998</v>
       </c>
       <c r="L61" s="107" t="s">
-        <v>997</v>
-      </c>
-      <c r="M61" s="107" t="s">
-        <v>998</v>
-      </c>
+        <v>999</v>
+      </c>
+      <c r="M61" s="107"/>
       <c r="N61" s="107"/>
       <c r="O61" s="107"/>
       <c r="P61" s="107"/>
@@ -16898,13 +16892,13 @@
       <c r="G62" s="107"/>
       <c r="H62" s="107"/>
       <c r="I62" s="107" t="s">
-        <v>999</v>
+        <v>1000</v>
       </c>
       <c r="J62" s="107" t="s">
-        <v>1000</v>
+        <v>1001</v>
       </c>
       <c r="K62" s="107" t="s">
-        <v>1001</v>
+        <v>1002</v>
       </c>
       <c r="L62" s="107"/>
       <c r="M62" s="107"/>
@@ -16936,13 +16930,13 @@
       <c r="G63" s="107"/>
       <c r="H63" s="107"/>
       <c r="I63" s="107" t="s">
-        <v>1002</v>
+        <v>1003</v>
       </c>
       <c r="J63" s="107" t="s">
-        <v>1003</v>
+        <v>1004</v>
       </c>
       <c r="K63" s="107" t="s">
-        <v>1004</v>
+        <v>1005</v>
       </c>
       <c r="L63" s="107"/>
       <c r="M63" s="107"/>
@@ -16974,7 +16968,7 @@
       <c r="G64" s="107"/>
       <c r="H64" s="107"/>
       <c r="I64" s="107" t="s">
-        <v>1005</v>
+        <v>1006</v>
       </c>
       <c r="J64" s="107" t="s">
         <v>1006</v>
@@ -17015,10 +17009,10 @@
         <v>1008</v>
       </c>
       <c r="J65" s="107" t="s">
-        <v>1008</v>
+        <v>1009</v>
       </c>
       <c r="K65" s="107" t="s">
-        <v>1009</v>
+        <v>1010</v>
       </c>
       <c r="L65" s="107"/>
       <c r="M65" s="107"/>
@@ -17050,15 +17044,17 @@
       <c r="G66" s="107"/>
       <c r="H66" s="107"/>
       <c r="I66" s="107" t="s">
-        <v>1010</v>
+        <v>1011</v>
       </c>
       <c r="J66" s="107" t="s">
-        <v>1011</v>
+        <v>1012</v>
       </c>
       <c r="K66" s="107" t="s">
-        <v>1012</v>
-      </c>
-      <c r="L66" s="107"/>
+        <v>1013</v>
+      </c>
+      <c r="L66" s="107" t="s">
+        <v>1014</v>
+      </c>
       <c r="M66" s="107"/>
       <c r="N66" s="107"/>
       <c r="O66" s="107"/>
@@ -17088,17 +17084,15 @@
       <c r="G67" s="107"/>
       <c r="H67" s="107"/>
       <c r="I67" s="107" t="s">
-        <v>1013</v>
+        <v>1015</v>
       </c>
       <c r="J67" s="107" t="s">
-        <v>1014</v>
+        <v>1016</v>
       </c>
       <c r="K67" s="107" t="s">
-        <v>1015</v>
-      </c>
-      <c r="L67" s="107" t="s">
-        <v>1016</v>
-      </c>
+        <v>1017</v>
+      </c>
+      <c r="L67" s="107"/>
       <c r="M67" s="107"/>
       <c r="N67" s="107"/>
       <c r="O67" s="107"/>
@@ -17128,13 +17122,13 @@
       <c r="G68" s="107"/>
       <c r="H68" s="107"/>
       <c r="I68" s="107" t="s">
-        <v>1017</v>
+        <v>1018</v>
       </c>
       <c r="J68" s="107" t="s">
-        <v>1018</v>
+        <v>1019</v>
       </c>
       <c r="K68" s="107" t="s">
-        <v>1019</v>
+        <v>1020</v>
       </c>
       <c r="L68" s="107"/>
       <c r="M68" s="107"/>
@@ -17166,7 +17160,7 @@
       <c r="G69" s="107"/>
       <c r="H69" s="107"/>
       <c r="I69" s="107" t="s">
-        <v>1020</v>
+        <v>1021</v>
       </c>
       <c r="J69" s="107" t="s">
         <v>1021</v>
@@ -17207,10 +17201,10 @@
         <v>1023</v>
       </c>
       <c r="J70" s="107" t="s">
-        <v>1023</v>
+        <v>1024</v>
       </c>
       <c r="K70" s="107" t="s">
-        <v>1024</v>
+        <v>1025</v>
       </c>
       <c r="L70" s="107"/>
       <c r="M70" s="107"/>
@@ -17242,13 +17236,13 @@
       <c r="G71" s="107"/>
       <c r="H71" s="107"/>
       <c r="I71" s="107" t="s">
-        <v>1025</v>
+        <v>1026</v>
       </c>
       <c r="J71" s="107" t="s">
-        <v>1026</v>
+        <v>1027</v>
       </c>
       <c r="K71" s="107" t="s">
-        <v>1027</v>
+        <v>1028</v>
       </c>
       <c r="L71" s="107"/>
       <c r="M71" s="107"/>
@@ -17280,7 +17274,7 @@
       <c r="G72" s="107"/>
       <c r="H72" s="107"/>
       <c r="I72" s="107" t="s">
-        <v>1028</v>
+        <v>1029</v>
       </c>
       <c r="J72" s="107" t="s">
         <v>1029</v>
@@ -17349,22 +17343,36 @@
     <row r="74" customFormat="false" ht="9.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A74" s="107"/>
       <c r="B74" s="107"/>
-      <c r="C74" s="107"/>
-      <c r="D74" s="107"/>
-      <c r="E74" s="107"/>
-      <c r="F74" s="107"/>
-      <c r="G74" s="107"/>
-      <c r="H74" s="107"/>
+      <c r="C74" s="115" t="s">
+        <v>1033</v>
+      </c>
+      <c r="D74" s="116" t="s">
+        <v>1034</v>
+      </c>
+      <c r="E74" s="116" t="s">
+        <v>1035</v>
+      </c>
+      <c r="F74" s="117" t="s">
+        <v>1036</v>
+      </c>
+      <c r="G74" s="107" t="s">
+        <v>1037</v>
+      </c>
+      <c r="H74" s="118" t="s">
+        <v>1038</v>
+      </c>
       <c r="I74" s="107" t="s">
-        <v>1033</v>
+        <v>1039</v>
       </c>
       <c r="J74" s="107" t="s">
-        <v>1033</v>
+        <v>1040</v>
       </c>
       <c r="K74" s="107" t="s">
-        <v>1034</v>
-      </c>
-      <c r="L74" s="107"/>
+        <v>1041</v>
+      </c>
+      <c r="L74" s="107" t="s">
+        <v>1042</v>
+      </c>
       <c r="M74" s="107"/>
       <c r="N74" s="107"/>
       <c r="O74" s="107"/>
@@ -17387,35 +17395,23 @@
     <row r="75" customFormat="false" ht="9.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A75" s="107"/>
       <c r="B75" s="107"/>
-      <c r="C75" s="115" t="s">
-        <v>1035</v>
-      </c>
-      <c r="D75" s="116" t="s">
-        <v>1036</v>
-      </c>
-      <c r="E75" s="116" t="s">
-        <v>1037</v>
-      </c>
-      <c r="F75" s="117" t="s">
-        <v>1038</v>
-      </c>
-      <c r="G75" s="107" t="s">
-        <v>1039</v>
-      </c>
-      <c r="H75" s="118" t="s">
-        <v>1040</v>
-      </c>
+      <c r="C75" s="107"/>
+      <c r="D75" s="107"/>
+      <c r="E75" s="107"/>
+      <c r="F75" s="107"/>
+      <c r="G75" s="107"/>
+      <c r="H75" s="107"/>
       <c r="I75" s="107" t="s">
-        <v>1041</v>
+        <v>1043</v>
       </c>
       <c r="J75" s="107" t="s">
-        <v>1042</v>
+        <v>1044</v>
       </c>
       <c r="K75" s="107" t="s">
-        <v>1043</v>
+        <v>1045</v>
       </c>
       <c r="L75" s="107" t="s">
-        <v>1044</v>
+        <v>1046</v>
       </c>
       <c r="M75" s="107"/>
       <c r="N75" s="107"/>
@@ -17446,16 +17442,16 @@
       <c r="G76" s="107"/>
       <c r="H76" s="107"/>
       <c r="I76" s="107" t="s">
-        <v>1045</v>
+        <v>1047</v>
       </c>
       <c r="J76" s="107" t="s">
-        <v>1046</v>
+        <v>1048</v>
       </c>
       <c r="K76" s="107" t="s">
-        <v>1047</v>
+        <v>1049</v>
       </c>
       <c r="L76" s="107" t="s">
-        <v>1048</v>
+        <v>1050</v>
       </c>
       <c r="M76" s="107"/>
       <c r="N76" s="107"/>
@@ -17486,16 +17482,16 @@
       <c r="G77" s="107"/>
       <c r="H77" s="107"/>
       <c r="I77" s="107" t="s">
-        <v>1049</v>
+        <v>1051</v>
       </c>
       <c r="J77" s="107" t="s">
-        <v>1050</v>
+        <v>1052</v>
       </c>
       <c r="K77" s="107" t="s">
-        <v>1051</v>
+        <v>1053</v>
       </c>
       <c r="L77" s="107" t="s">
-        <v>1052</v>
+        <v>1054</v>
       </c>
       <c r="M77" s="107"/>
       <c r="N77" s="107"/>
@@ -17526,16 +17522,16 @@
       <c r="G78" s="107"/>
       <c r="H78" s="107"/>
       <c r="I78" s="107" t="s">
-        <v>1053</v>
+        <v>1055</v>
       </c>
       <c r="J78" s="107" t="s">
-        <v>1054</v>
+        <v>1056</v>
       </c>
       <c r="K78" s="107" t="s">
-        <v>1055</v>
+        <v>1057</v>
       </c>
       <c r="L78" s="107" t="s">
-        <v>1056</v>
+        <v>1058</v>
       </c>
       <c r="M78" s="107"/>
       <c r="N78" s="107"/>
@@ -17566,16 +17562,16 @@
       <c r="G79" s="107"/>
       <c r="H79" s="107"/>
       <c r="I79" s="107" t="s">
-        <v>1057</v>
+        <v>1059</v>
       </c>
       <c r="J79" s="107" t="s">
-        <v>1058</v>
+        <v>1059</v>
       </c>
       <c r="K79" s="107" t="s">
-        <v>1059</v>
+        <v>1060</v>
       </c>
       <c r="L79" s="107" t="s">
-        <v>1060</v>
+        <v>1061</v>
       </c>
       <c r="M79" s="107"/>
       <c r="N79" s="107"/>
@@ -17606,16 +17602,16 @@
       <c r="G80" s="107"/>
       <c r="H80" s="107"/>
       <c r="I80" s="107" t="s">
-        <v>1061</v>
+        <v>1062</v>
       </c>
       <c r="J80" s="107" t="s">
-        <v>1061</v>
+        <v>1062</v>
       </c>
       <c r="K80" s="107" t="s">
-        <v>1062</v>
+        <v>1063</v>
       </c>
       <c r="L80" s="107" t="s">
-        <v>1063</v>
+        <v>1064</v>
       </c>
       <c r="M80" s="107"/>
       <c r="N80" s="107"/>
@@ -17646,16 +17642,16 @@
       <c r="G81" s="107"/>
       <c r="H81" s="107"/>
       <c r="I81" s="107" t="s">
-        <v>1064</v>
+        <v>1065</v>
       </c>
       <c r="J81" s="107" t="s">
-        <v>1064</v>
+        <v>1065</v>
       </c>
       <c r="K81" s="107" t="s">
-        <v>1065</v>
+        <v>1066</v>
       </c>
       <c r="L81" s="107" t="s">
-        <v>1066</v>
+        <v>1067</v>
       </c>
       <c r="M81" s="107"/>
       <c r="N81" s="107"/>
@@ -17686,16 +17682,16 @@
       <c r="G82" s="107"/>
       <c r="H82" s="107"/>
       <c r="I82" s="107" t="s">
-        <v>1067</v>
+        <v>1068</v>
       </c>
       <c r="J82" s="107" t="s">
-        <v>1067</v>
+        <v>1069</v>
       </c>
       <c r="K82" s="107" t="s">
-        <v>1068</v>
+        <v>1070</v>
       </c>
       <c r="L82" s="107" t="s">
-        <v>1069</v>
+        <v>1071</v>
       </c>
       <c r="M82" s="107"/>
       <c r="N82" s="107"/>
@@ -17726,16 +17722,16 @@
       <c r="G83" s="107"/>
       <c r="H83" s="107"/>
       <c r="I83" s="107" t="s">
-        <v>1070</v>
+        <v>1072</v>
       </c>
       <c r="J83" s="107" t="s">
-        <v>1071</v>
+        <v>1073</v>
       </c>
       <c r="K83" s="107" t="s">
-        <v>1072</v>
+        <v>1074</v>
       </c>
       <c r="L83" s="107" t="s">
-        <v>1073</v>
+        <v>1075</v>
       </c>
       <c r="M83" s="107"/>
       <c r="N83" s="107"/>
@@ -17766,17 +17762,15 @@
       <c r="G84" s="107"/>
       <c r="H84" s="107"/>
       <c r="I84" s="107" t="s">
-        <v>1074</v>
+        <v>1076</v>
       </c>
       <c r="J84" s="107" t="s">
-        <v>1075</v>
+        <v>1076</v>
       </c>
       <c r="K84" s="107" t="s">
-        <v>1076</v>
-      </c>
-      <c r="L84" s="107" t="s">
         <v>1077</v>
       </c>
+      <c r="L84" s="107"/>
       <c r="M84" s="107"/>
       <c r="N84" s="107"/>
       <c r="O84" s="107"/>
@@ -17879,16 +17873,20 @@
       <c r="D87" s="107"/>
       <c r="E87" s="107"/>
       <c r="F87" s="107"/>
-      <c r="G87" s="107"/>
-      <c r="H87" s="107"/>
+      <c r="G87" s="107" t="s">
+        <v>1082</v>
+      </c>
+      <c r="H87" s="118" t="s">
+        <v>1083</v>
+      </c>
       <c r="I87" s="107" t="s">
-        <v>1082</v>
+        <v>1084</v>
       </c>
       <c r="J87" s="107" t="s">
-        <v>1082</v>
+        <v>1085</v>
       </c>
       <c r="K87" s="107" t="s">
-        <v>1083</v>
+        <v>1086</v>
       </c>
       <c r="L87" s="107"/>
       <c r="M87" s="107"/>
@@ -17917,17 +17915,13 @@
       <c r="D88" s="107"/>
       <c r="E88" s="107"/>
       <c r="F88" s="107"/>
-      <c r="G88" s="107" t="s">
-        <v>1084</v>
-      </c>
-      <c r="H88" s="118" t="s">
+      <c r="G88" s="107"/>
+      <c r="H88" s="107"/>
+      <c r="I88" s="107" t="s">
+        <v>1087</v>
+      </c>
+      <c r="J88" s="107" t="s">
         <v>1085</v>
-      </c>
-      <c r="I88" s="107" t="s">
-        <v>1086</v>
-      </c>
-      <c r="J88" s="107" t="s">
-        <v>1087</v>
       </c>
       <c r="K88" s="107" t="s">
         <v>1088</v>
@@ -17965,7 +17959,7 @@
         <v>1089</v>
       </c>
       <c r="J89" s="107" t="s">
-        <v>1087</v>
+        <v>1085</v>
       </c>
       <c r="K89" s="107" t="s">
         <v>1090</v>
@@ -18003,7 +17997,7 @@
         <v>1091</v>
       </c>
       <c r="J90" s="107" t="s">
-        <v>1087</v>
+        <v>1085</v>
       </c>
       <c r="K90" s="107" t="s">
         <v>1092</v>
@@ -18041,7 +18035,7 @@
         <v>1093</v>
       </c>
       <c r="J91" s="107" t="s">
-        <v>1087</v>
+        <v>1085</v>
       </c>
       <c r="K91" s="107" t="s">
         <v>1094</v>
@@ -18079,10 +18073,10 @@
         <v>1095</v>
       </c>
       <c r="J92" s="107" t="s">
-        <v>1087</v>
+        <v>1096</v>
       </c>
       <c r="K92" s="107" t="s">
-        <v>1096</v>
+        <v>1097</v>
       </c>
       <c r="L92" s="107"/>
       <c r="M92" s="107"/>
@@ -18114,13 +18108,13 @@
       <c r="G93" s="107"/>
       <c r="H93" s="107"/>
       <c r="I93" s="107" t="s">
-        <v>1097</v>
+        <v>1098</v>
       </c>
       <c r="J93" s="107" t="s">
-        <v>1098</v>
+        <v>1099</v>
       </c>
       <c r="K93" s="107" t="s">
-        <v>1099</v>
+        <v>1100</v>
       </c>
       <c r="L93" s="107"/>
       <c r="M93" s="107"/>
@@ -18152,13 +18146,13 @@
       <c r="G94" s="107"/>
       <c r="H94" s="107"/>
       <c r="I94" s="107" t="s">
-        <v>1100</v>
+        <v>1101</v>
       </c>
       <c r="J94" s="107" t="s">
-        <v>1101</v>
+        <v>1102</v>
       </c>
       <c r="K94" s="107" t="s">
-        <v>1102</v>
+        <v>1103</v>
       </c>
       <c r="L94" s="107"/>
       <c r="M94" s="107"/>
@@ -18187,16 +18181,20 @@
       <c r="D95" s="107"/>
       <c r="E95" s="107"/>
       <c r="F95" s="107"/>
-      <c r="G95" s="107"/>
-      <c r="H95" s="107"/>
+      <c r="G95" s="107" t="s">
+        <v>1104</v>
+      </c>
+      <c r="H95" s="118" t="s">
+        <v>1105</v>
+      </c>
       <c r="I95" s="107" t="s">
-        <v>1103</v>
+        <v>1106</v>
       </c>
       <c r="J95" s="107" t="s">
-        <v>1104</v>
+        <v>1107</v>
       </c>
       <c r="K95" s="107" t="s">
-        <v>1105</v>
+        <v>1108</v>
       </c>
       <c r="L95" s="107"/>
       <c r="M95" s="107"/>
@@ -18225,20 +18223,16 @@
       <c r="D96" s="107"/>
       <c r="E96" s="107"/>
       <c r="F96" s="107"/>
-      <c r="G96" s="107" t="s">
-        <v>1106</v>
-      </c>
-      <c r="H96" s="118" t="s">
-        <v>1107</v>
-      </c>
+      <c r="G96" s="107"/>
+      <c r="H96" s="107"/>
       <c r="I96" s="107" t="s">
-        <v>1108</v>
+        <v>1109</v>
       </c>
       <c r="J96" s="107" t="s">
-        <v>1109</v>
+        <v>1110</v>
       </c>
       <c r="K96" s="107" t="s">
-        <v>1110</v>
+        <v>1111</v>
       </c>
       <c r="L96" s="107"/>
       <c r="M96" s="107"/>
@@ -18270,13 +18264,13 @@
       <c r="G97" s="107"/>
       <c r="H97" s="107"/>
       <c r="I97" s="107" t="s">
-        <v>1111</v>
+        <v>1112</v>
       </c>
       <c r="J97" s="107" t="s">
-        <v>1112</v>
+        <v>1113</v>
       </c>
       <c r="K97" s="107" t="s">
-        <v>1113</v>
+        <v>1114</v>
       </c>
       <c r="L97" s="107"/>
       <c r="M97" s="107"/>
@@ -18308,13 +18302,13 @@
       <c r="G98" s="107"/>
       <c r="H98" s="107"/>
       <c r="I98" s="107" t="s">
-        <v>1114</v>
+        <v>1115</v>
       </c>
       <c r="J98" s="107" t="s">
-        <v>1115</v>
+        <v>1116</v>
       </c>
       <c r="K98" s="107" t="s">
-        <v>1116</v>
+        <v>1117</v>
       </c>
       <c r="L98" s="107"/>
       <c r="M98" s="107"/>
@@ -18346,13 +18340,13 @@
       <c r="G99" s="107"/>
       <c r="H99" s="107"/>
       <c r="I99" s="107" t="s">
-        <v>1117</v>
+        <v>1118</v>
       </c>
       <c r="J99" s="107" t="s">
-        <v>1118</v>
+        <v>1119</v>
       </c>
       <c r="K99" s="107" t="s">
-        <v>1119</v>
+        <v>1120</v>
       </c>
       <c r="L99" s="107"/>
       <c r="M99" s="107"/>
@@ -18384,13 +18378,13 @@
       <c r="G100" s="107"/>
       <c r="H100" s="107"/>
       <c r="I100" s="107" t="s">
-        <v>1120</v>
+        <v>1121</v>
       </c>
       <c r="J100" s="107" t="s">
-        <v>1121</v>
+        <v>1122</v>
       </c>
       <c r="K100" s="107" t="s">
-        <v>1122</v>
+        <v>1123</v>
       </c>
       <c r="L100" s="107"/>
       <c r="M100" s="107"/>
@@ -18422,13 +18416,13 @@
       <c r="G101" s="107"/>
       <c r="H101" s="107"/>
       <c r="I101" s="107" t="s">
-        <v>1123</v>
+        <v>1124</v>
       </c>
       <c r="J101" s="107" t="s">
-        <v>1124</v>
+        <v>1125</v>
       </c>
       <c r="K101" s="107" t="s">
-        <v>1125</v>
+        <v>1126</v>
       </c>
       <c r="L101" s="107"/>
       <c r="M101" s="107"/>
@@ -18460,13 +18454,13 @@
       <c r="G102" s="107"/>
       <c r="H102" s="107"/>
       <c r="I102" s="107" t="s">
-        <v>1126</v>
+        <v>1127</v>
       </c>
       <c r="J102" s="107" t="s">
-        <v>1127</v>
+        <v>1128</v>
       </c>
       <c r="K102" s="107" t="s">
-        <v>1128</v>
+        <v>1129</v>
       </c>
       <c r="L102" s="107"/>
       <c r="M102" s="107"/>
@@ -18498,13 +18492,13 @@
       <c r="G103" s="107"/>
       <c r="H103" s="107"/>
       <c r="I103" s="107" t="s">
-        <v>1129</v>
+        <v>1130</v>
       </c>
       <c r="J103" s="107" t="s">
-        <v>1130</v>
+        <v>1131</v>
       </c>
       <c r="K103" s="107" t="s">
-        <v>1131</v>
+        <v>1132</v>
       </c>
       <c r="L103" s="107"/>
       <c r="M103" s="107"/>
@@ -18536,13 +18530,13 @@
       <c r="G104" s="107"/>
       <c r="H104" s="107"/>
       <c r="I104" s="107" t="s">
-        <v>1132</v>
+        <v>1133</v>
       </c>
       <c r="J104" s="107" t="s">
-        <v>1133</v>
+        <v>1134</v>
       </c>
       <c r="K104" s="107" t="s">
-        <v>1134</v>
+        <v>1135</v>
       </c>
       <c r="L104" s="107"/>
       <c r="M104" s="107"/>
@@ -18569,18 +18563,26 @@
       <c r="B105" s="107"/>
       <c r="C105" s="107"/>
       <c r="D105" s="107"/>
-      <c r="E105" s="107"/>
-      <c r="F105" s="107"/>
-      <c r="G105" s="107"/>
-      <c r="H105" s="107"/>
+      <c r="E105" s="116" t="s">
+        <v>1136</v>
+      </c>
+      <c r="F105" s="116" t="s">
+        <v>1137</v>
+      </c>
+      <c r="G105" s="107" t="s">
+        <v>1138</v>
+      </c>
+      <c r="H105" s="118" t="s">
+        <v>1139</v>
+      </c>
       <c r="I105" s="107" t="s">
-        <v>1135</v>
+        <v>1138</v>
       </c>
       <c r="J105" s="107" t="s">
-        <v>1136</v>
+        <v>1140</v>
       </c>
       <c r="K105" s="107" t="s">
-        <v>1137</v>
+        <v>1141</v>
       </c>
       <c r="L105" s="107"/>
       <c r="M105" s="107"/>
@@ -18607,26 +18609,22 @@
       <c r="B106" s="107"/>
       <c r="C106" s="107"/>
       <c r="D106" s="107"/>
-      <c r="E106" s="116" t="s">
-        <v>1138</v>
-      </c>
-      <c r="F106" s="116" t="s">
-        <v>1139</v>
-      </c>
+      <c r="E106" s="107"/>
+      <c r="F106" s="107"/>
       <c r="G106" s="107" t="s">
-        <v>1140</v>
+        <v>1142</v>
       </c>
       <c r="H106" s="118" t="s">
-        <v>1141</v>
+        <v>1143</v>
       </c>
       <c r="I106" s="107" t="s">
-        <v>1140</v>
+        <v>1144</v>
       </c>
       <c r="J106" s="107" t="s">
-        <v>1142</v>
+        <v>1145</v>
       </c>
       <c r="K106" s="107" t="s">
-        <v>1143</v>
+        <v>1146</v>
       </c>
       <c r="L106" s="107"/>
       <c r="M106" s="107"/>
@@ -18655,20 +18653,16 @@
       <c r="D107" s="107"/>
       <c r="E107" s="107"/>
       <c r="F107" s="107"/>
-      <c r="G107" s="107" t="s">
-        <v>1144</v>
-      </c>
-      <c r="H107" s="118" t="s">
-        <v>1145</v>
-      </c>
+      <c r="G107" s="107"/>
+      <c r="H107" s="107"/>
       <c r="I107" s="107" t="s">
-        <v>1146</v>
+        <v>1147</v>
       </c>
       <c r="J107" s="107" t="s">
-        <v>1147</v>
+        <v>1148</v>
       </c>
       <c r="K107" s="107" t="s">
-        <v>1148</v>
+        <v>1149</v>
       </c>
       <c r="L107" s="107"/>
       <c r="M107" s="107"/>
@@ -18700,13 +18694,13 @@
       <c r="G108" s="107"/>
       <c r="H108" s="107"/>
       <c r="I108" s="107" t="s">
-        <v>1149</v>
+        <v>1150</v>
       </c>
       <c r="J108" s="107" t="s">
-        <v>1150</v>
+        <v>1151</v>
       </c>
       <c r="K108" s="107" t="s">
-        <v>1151</v>
+        <v>1152</v>
       </c>
       <c r="L108" s="107"/>
       <c r="M108" s="107"/>
@@ -18738,13 +18732,13 @@
       <c r="G109" s="107"/>
       <c r="H109" s="107"/>
       <c r="I109" s="107" t="s">
-        <v>1152</v>
+        <v>1153</v>
       </c>
       <c r="J109" s="107" t="s">
-        <v>1153</v>
+        <v>1154</v>
       </c>
       <c r="K109" s="107" t="s">
-        <v>1154</v>
+        <v>1155</v>
       </c>
       <c r="L109" s="107"/>
       <c r="M109" s="107"/>
@@ -18776,13 +18770,13 @@
       <c r="G110" s="107"/>
       <c r="H110" s="107"/>
       <c r="I110" s="107" t="s">
-        <v>1155</v>
+        <v>1156</v>
       </c>
       <c r="J110" s="107" t="s">
-        <v>1156</v>
+        <v>1157</v>
       </c>
       <c r="K110" s="107" t="s">
-        <v>1157</v>
+        <v>1158</v>
       </c>
       <c r="L110" s="107"/>
       <c r="M110" s="107"/>
@@ -18811,16 +18805,20 @@
       <c r="D111" s="107"/>
       <c r="E111" s="107"/>
       <c r="F111" s="107"/>
-      <c r="G111" s="107"/>
-      <c r="H111" s="107"/>
+      <c r="G111" s="107" t="s">
+        <v>1159</v>
+      </c>
+      <c r="H111" s="118" t="s">
+        <v>1160</v>
+      </c>
       <c r="I111" s="107" t="s">
-        <v>1158</v>
+        <v>1161</v>
       </c>
       <c r="J111" s="107" t="s">
-        <v>1159</v>
+        <v>1162</v>
       </c>
       <c r="K111" s="107" t="s">
-        <v>1160</v>
+        <v>1163</v>
       </c>
       <c r="L111" s="107"/>
       <c r="M111" s="107"/>
@@ -18849,20 +18847,16 @@
       <c r="D112" s="107"/>
       <c r="E112" s="107"/>
       <c r="F112" s="107"/>
-      <c r="G112" s="107" t="s">
-        <v>1161</v>
-      </c>
-      <c r="H112" s="118" t="s">
-        <v>1162</v>
-      </c>
+      <c r="G112" s="107"/>
+      <c r="H112" s="107"/>
       <c r="I112" s="107" t="s">
-        <v>1163</v>
+        <v>1164</v>
       </c>
       <c r="J112" s="107" t="s">
-        <v>1164</v>
+        <v>1165</v>
       </c>
       <c r="K112" s="107" t="s">
-        <v>1165</v>
+        <v>1166</v>
       </c>
       <c r="L112" s="107"/>
       <c r="M112" s="107"/>
@@ -18894,13 +18888,13 @@
       <c r="G113" s="107"/>
       <c r="H113" s="107"/>
       <c r="I113" s="107" t="s">
-        <v>1166</v>
+        <v>1167</v>
       </c>
       <c r="J113" s="107" t="s">
-        <v>1167</v>
+        <v>1168</v>
       </c>
       <c r="K113" s="107" t="s">
-        <v>1168</v>
+        <v>1169</v>
       </c>
       <c r="L113" s="107"/>
       <c r="M113" s="107"/>
@@ -18932,13 +18926,13 @@
       <c r="G114" s="107"/>
       <c r="H114" s="107"/>
       <c r="I114" s="107" t="s">
-        <v>1169</v>
+        <v>1170</v>
       </c>
       <c r="J114" s="107" t="s">
-        <v>1170</v>
+        <v>1171</v>
       </c>
       <c r="K114" s="107" t="s">
-        <v>1171</v>
+        <v>1172</v>
       </c>
       <c r="L114" s="107"/>
       <c r="M114" s="107"/>
@@ -18970,13 +18964,13 @@
       <c r="G115" s="107"/>
       <c r="H115" s="107"/>
       <c r="I115" s="107" t="s">
-        <v>1172</v>
+        <v>1173</v>
       </c>
       <c r="J115" s="107" t="s">
-        <v>1173</v>
+        <v>1174</v>
       </c>
       <c r="K115" s="107" t="s">
-        <v>1174</v>
+        <v>1175</v>
       </c>
       <c r="L115" s="107"/>
       <c r="M115" s="107"/>
@@ -19008,13 +19002,13 @@
       <c r="G116" s="107"/>
       <c r="H116" s="107"/>
       <c r="I116" s="107" t="s">
-        <v>1175</v>
+        <v>1176</v>
       </c>
       <c r="J116" s="107" t="s">
-        <v>1176</v>
+        <v>1177</v>
       </c>
       <c r="K116" s="107" t="s">
-        <v>1177</v>
+        <v>1178</v>
       </c>
       <c r="L116" s="107"/>
       <c r="M116" s="107"/>
@@ -19046,13 +19040,13 @@
       <c r="G117" s="107"/>
       <c r="H117" s="107"/>
       <c r="I117" s="107" t="s">
-        <v>1178</v>
+        <v>1179</v>
       </c>
       <c r="J117" s="107" t="s">
-        <v>1179</v>
+        <v>1180</v>
       </c>
       <c r="K117" s="107" t="s">
-        <v>1180</v>
+        <v>1181</v>
       </c>
       <c r="L117" s="107"/>
       <c r="M117" s="107"/>
@@ -19084,13 +19078,13 @@
       <c r="G118" s="107"/>
       <c r="H118" s="107"/>
       <c r="I118" s="107" t="s">
-        <v>1181</v>
+        <v>1182</v>
       </c>
       <c r="J118" s="107" t="s">
-        <v>1182</v>
+        <v>1183</v>
       </c>
       <c r="K118" s="107" t="s">
-        <v>1183</v>
+        <v>1184</v>
       </c>
       <c r="L118" s="107"/>
       <c r="M118" s="107"/>
@@ -19122,13 +19116,13 @@
       <c r="G119" s="107"/>
       <c r="H119" s="107"/>
       <c r="I119" s="107" t="s">
-        <v>1184</v>
+        <v>1185</v>
       </c>
       <c r="J119" s="107" t="s">
-        <v>1185</v>
+        <v>1186</v>
       </c>
       <c r="K119" s="107" t="s">
-        <v>1186</v>
+        <v>1187</v>
       </c>
       <c r="L119" s="107"/>
       <c r="M119" s="107"/>
@@ -19160,13 +19154,13 @@
       <c r="G120" s="107"/>
       <c r="H120" s="107"/>
       <c r="I120" s="107" t="s">
-        <v>1187</v>
+        <v>1188</v>
       </c>
       <c r="J120" s="107" t="s">
-        <v>1188</v>
+        <v>1189</v>
       </c>
       <c r="K120" s="107" t="s">
-        <v>1189</v>
+        <v>1190</v>
       </c>
       <c r="L120" s="107"/>
       <c r="M120" s="107"/>
@@ -19198,13 +19192,13 @@
       <c r="G121" s="107"/>
       <c r="H121" s="107"/>
       <c r="I121" s="107" t="s">
-        <v>1190</v>
+        <v>1191</v>
       </c>
       <c r="J121" s="107" t="s">
-        <v>1191</v>
+        <v>1192</v>
       </c>
       <c r="K121" s="107" t="s">
-        <v>1192</v>
+        <v>1193</v>
       </c>
       <c r="L121" s="107"/>
       <c r="M121" s="107"/>
@@ -19236,13 +19230,13 @@
       <c r="G122" s="107"/>
       <c r="H122" s="107"/>
       <c r="I122" s="107" t="s">
-        <v>1193</v>
+        <v>1194</v>
       </c>
       <c r="J122" s="107" t="s">
-        <v>1194</v>
+        <v>1195</v>
       </c>
       <c r="K122" s="107" t="s">
-        <v>1195</v>
+        <v>1196</v>
       </c>
       <c r="L122" s="107"/>
       <c r="M122" s="107"/>
@@ -19271,16 +19265,20 @@
       <c r="D123" s="107"/>
       <c r="E123" s="107"/>
       <c r="F123" s="107"/>
-      <c r="G123" s="107"/>
-      <c r="H123" s="107"/>
+      <c r="G123" s="107" t="s">
+        <v>1197</v>
+      </c>
+      <c r="H123" s="118" t="s">
+        <v>1198</v>
+      </c>
       <c r="I123" s="107" t="s">
-        <v>1196</v>
+        <v>1199</v>
       </c>
       <c r="J123" s="107" t="s">
-        <v>1197</v>
+        <v>1200</v>
       </c>
       <c r="K123" s="107" t="s">
-        <v>1198</v>
+        <v>1201</v>
       </c>
       <c r="L123" s="107"/>
       <c r="M123" s="107"/>
@@ -19309,20 +19307,16 @@
       <c r="D124" s="107"/>
       <c r="E124" s="107"/>
       <c r="F124" s="107"/>
-      <c r="G124" s="107" t="s">
-        <v>1199</v>
-      </c>
-      <c r="H124" s="118" t="s">
-        <v>1200</v>
-      </c>
+      <c r="G124" s="107"/>
+      <c r="H124" s="107"/>
       <c r="I124" s="107" t="s">
-        <v>1201</v>
+        <v>1202</v>
       </c>
       <c r="J124" s="107" t="s">
-        <v>1202</v>
+        <v>1203</v>
       </c>
       <c r="K124" s="107" t="s">
-        <v>1203</v>
+        <v>1204</v>
       </c>
       <c r="L124" s="107"/>
       <c r="M124" s="107"/>
@@ -19354,13 +19348,13 @@
       <c r="G125" s="107"/>
       <c r="H125" s="107"/>
       <c r="I125" s="107" t="s">
-        <v>1204</v>
+        <v>1205</v>
       </c>
       <c r="J125" s="107" t="s">
-        <v>1205</v>
+        <v>1206</v>
       </c>
       <c r="K125" s="107" t="s">
-        <v>1206</v>
+        <v>1207</v>
       </c>
       <c r="L125" s="107"/>
       <c r="M125" s="107"/>
@@ -19392,13 +19386,13 @@
       <c r="G126" s="107"/>
       <c r="H126" s="107"/>
       <c r="I126" s="107" t="s">
-        <v>1207</v>
+        <v>1208</v>
       </c>
       <c r="J126" s="107" t="s">
-        <v>1208</v>
+        <v>1209</v>
       </c>
       <c r="K126" s="107" t="s">
-        <v>1209</v>
+        <v>1210</v>
       </c>
       <c r="L126" s="107"/>
       <c r="M126" s="107"/>
@@ -19430,13 +19424,13 @@
       <c r="G127" s="107"/>
       <c r="H127" s="107"/>
       <c r="I127" s="107" t="s">
-        <v>1210</v>
+        <v>1211</v>
       </c>
       <c r="J127" s="107" t="s">
-        <v>1211</v>
+        <v>1212</v>
       </c>
       <c r="K127" s="107" t="s">
-        <v>1212</v>
+        <v>1213</v>
       </c>
       <c r="L127" s="107"/>
       <c r="M127" s="107"/>
@@ -19461,21 +19455,27 @@
     <row r="128" customFormat="false" ht="9.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A128" s="107"/>
       <c r="B128" s="107"/>
-      <c r="C128" s="107"/>
-      <c r="D128" s="107"/>
-      <c r="E128" s="107"/>
-      <c r="F128" s="107"/>
-      <c r="G128" s="107"/>
-      <c r="H128" s="107"/>
-      <c r="I128" s="107" t="s">
-        <v>1213</v>
-      </c>
-      <c r="J128" s="107" t="s">
+      <c r="C128" s="111" t="s">
         <v>1214</v>
       </c>
-      <c r="K128" s="107" t="s">
+      <c r="D128" s="108" t="s">
         <v>1215</v>
       </c>
+      <c r="E128" s="111" t="s">
+        <v>1216</v>
+      </c>
+      <c r="F128" s="108" t="s">
+        <v>1217</v>
+      </c>
+      <c r="G128" s="107" t="s">
+        <v>1218</v>
+      </c>
+      <c r="H128" s="118" t="s">
+        <v>1219</v>
+      </c>
+      <c r="I128" s="107"/>
+      <c r="J128" s="107"/>
+      <c r="K128" s="107"/>
       <c r="L128" s="107"/>
       <c r="M128" s="107"/>
       <c r="N128" s="107"/>
@@ -19499,27 +19499,21 @@
     <row r="129" customFormat="false" ht="9.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A129" s="107"/>
       <c r="B129" s="107"/>
-      <c r="C129" s="111" t="s">
-        <v>1216</v>
-      </c>
-      <c r="D129" s="108" t="s">
-        <v>1217</v>
-      </c>
-      <c r="E129" s="111" t="s">
-        <v>1218</v>
-      </c>
-      <c r="F129" s="108" t="s">
-        <v>1219</v>
-      </c>
-      <c r="G129" s="107" t="s">
+      <c r="C129" s="107"/>
+      <c r="D129" s="107"/>
+      <c r="E129" s="107"/>
+      <c r="F129" s="107"/>
+      <c r="G129" s="107"/>
+      <c r="H129" s="107"/>
+      <c r="I129" s="107" t="s">
         <v>1220</v>
       </c>
-      <c r="H129" s="118" t="s">
+      <c r="J129" s="107" t="s">
         <v>1221</v>
       </c>
-      <c r="I129" s="107"/>
-      <c r="J129" s="107"/>
-      <c r="K129" s="107"/>
+      <c r="K129" s="107" t="s">
+        <v>1222</v>
+      </c>
       <c r="L129" s="107"/>
       <c r="M129" s="107"/>
       <c r="N129" s="107"/>
@@ -19550,13 +19544,13 @@
       <c r="G130" s="107"/>
       <c r="H130" s="107"/>
       <c r="I130" s="107" t="s">
-        <v>1222</v>
+        <v>1223</v>
       </c>
       <c r="J130" s="107" t="s">
-        <v>1223</v>
+        <v>1224</v>
       </c>
       <c r="K130" s="107" t="s">
-        <v>1224</v>
+        <v>1225</v>
       </c>
       <c r="L130" s="107"/>
       <c r="M130" s="107"/>
@@ -19588,13 +19582,13 @@
       <c r="G131" s="107"/>
       <c r="H131" s="107"/>
       <c r="I131" s="107" t="s">
-        <v>1225</v>
+        <v>1226</v>
       </c>
       <c r="J131" s="107" t="s">
-        <v>1226</v>
+        <v>1227</v>
       </c>
       <c r="K131" s="107" t="s">
-        <v>1227</v>
+        <v>1228</v>
       </c>
       <c r="L131" s="107"/>
       <c r="M131" s="107"/>
@@ -19626,13 +19620,13 @@
       <c r="G132" s="107"/>
       <c r="H132" s="107"/>
       <c r="I132" s="107" t="s">
-        <v>1228</v>
+        <v>1229</v>
       </c>
       <c r="J132" s="107" t="s">
-        <v>1229</v>
+        <v>1230</v>
       </c>
       <c r="K132" s="107" t="s">
-        <v>1230</v>
+        <v>1231</v>
       </c>
       <c r="L132" s="107"/>
       <c r="M132" s="107"/>
@@ -19664,13 +19658,13 @@
       <c r="G133" s="107"/>
       <c r="H133" s="107"/>
       <c r="I133" s="107" t="s">
-        <v>1231</v>
+        <v>1232</v>
       </c>
       <c r="J133" s="107" t="s">
-        <v>1232</v>
+        <v>1233</v>
       </c>
       <c r="K133" s="107" t="s">
-        <v>1233</v>
+        <v>1234</v>
       </c>
       <c r="L133" s="107"/>
       <c r="M133" s="107"/>
@@ -19702,13 +19696,13 @@
       <c r="G134" s="107"/>
       <c r="H134" s="107"/>
       <c r="I134" s="107" t="s">
-        <v>1234</v>
+        <v>1235</v>
       </c>
       <c r="J134" s="107" t="s">
-        <v>1235</v>
+        <v>1236</v>
       </c>
       <c r="K134" s="107" t="s">
-        <v>1236</v>
+        <v>1237</v>
       </c>
       <c r="L134" s="107"/>
       <c r="M134" s="107"/>
@@ -19740,13 +19734,13 @@
       <c r="G135" s="107"/>
       <c r="H135" s="107"/>
       <c r="I135" s="107" t="s">
-        <v>1237</v>
+        <v>1238</v>
       </c>
       <c r="J135" s="107" t="s">
-        <v>1238</v>
+        <v>1239</v>
       </c>
       <c r="K135" s="107" t="s">
-        <v>1239</v>
+        <v>1240</v>
       </c>
       <c r="L135" s="107"/>
       <c r="M135" s="107"/>
@@ -19778,13 +19772,13 @@
       <c r="G136" s="107"/>
       <c r="H136" s="107"/>
       <c r="I136" s="107" t="s">
-        <v>1240</v>
+        <v>1241</v>
       </c>
       <c r="J136" s="107" t="s">
-        <v>1241</v>
+        <v>1242</v>
       </c>
       <c r="K136" s="107" t="s">
-        <v>1242</v>
+        <v>1243</v>
       </c>
       <c r="L136" s="107"/>
       <c r="M136" s="107"/>
@@ -19813,19 +19807,27 @@
       <c r="D137" s="107"/>
       <c r="E137" s="107"/>
       <c r="F137" s="107"/>
-      <c r="G137" s="107"/>
-      <c r="H137" s="107"/>
+      <c r="G137" s="107" t="s">
+        <v>1244</v>
+      </c>
+      <c r="H137" s="118" t="s">
+        <v>1245</v>
+      </c>
       <c r="I137" s="107" t="s">
-        <v>1243</v>
+        <v>1246</v>
       </c>
       <c r="J137" s="107" t="s">
-        <v>1244</v>
+        <v>1247</v>
       </c>
       <c r="K137" s="107" t="s">
-        <v>1245</v>
-      </c>
-      <c r="L137" s="107"/>
-      <c r="M137" s="107"/>
+        <v>1248</v>
+      </c>
+      <c r="L137" s="107" t="s">
+        <v>1249</v>
+      </c>
+      <c r="M137" s="107" t="s">
+        <v>1250</v>
+      </c>
       <c r="N137" s="107"/>
       <c r="O137" s="107"/>
       <c r="P137" s="107"/>
@@ -19842,7 +19844,9 @@
       <c r="AA137" s="107"/>
       <c r="AB137" s="107"/>
       <c r="AC137" s="107"/>
-      <c r="AD137" s="107"/>
+      <c r="AD137" s="107" t="s">
+        <v>1244</v>
+      </c>
     </row>
     <row r="138" customFormat="false" ht="9.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A138" s="107"/>
@@ -19851,26 +19855,22 @@
       <c r="D138" s="107"/>
       <c r="E138" s="107"/>
       <c r="F138" s="107"/>
-      <c r="G138" s="107" t="s">
-        <v>1246</v>
-      </c>
-      <c r="H138" s="118" t="s">
-        <v>1247</v>
-      </c>
+      <c r="G138" s="107"/>
+      <c r="H138" s="107"/>
       <c r="I138" s="107" t="s">
-        <v>1248</v>
+        <v>1251</v>
       </c>
       <c r="J138" s="107" t="s">
-        <v>1249</v>
+        <v>1252</v>
       </c>
       <c r="K138" s="107" t="s">
-        <v>1250</v>
+        <v>1253</v>
       </c>
       <c r="L138" s="107" t="s">
-        <v>1251</v>
+        <v>1254</v>
       </c>
       <c r="M138" s="107" t="s">
-        <v>1252</v>
+        <v>1255</v>
       </c>
       <c r="N138" s="107"/>
       <c r="O138" s="107"/>
@@ -19888,9 +19888,7 @@
       <c r="AA138" s="107"/>
       <c r="AB138" s="107"/>
       <c r="AC138" s="107"/>
-      <c r="AD138" s="107" t="s">
-        <v>1246</v>
-      </c>
+      <c r="AD138" s="107"/>
     </row>
     <row r="139" customFormat="false" ht="9.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A139" s="107"/>
@@ -19902,19 +19900,19 @@
       <c r="G139" s="107"/>
       <c r="H139" s="107"/>
       <c r="I139" s="107" t="s">
-        <v>1253</v>
+        <v>1256</v>
       </c>
       <c r="J139" s="107" t="s">
-        <v>1254</v>
+        <v>1257</v>
       </c>
       <c r="K139" s="107" t="s">
-        <v>1255</v>
+        <v>1258</v>
       </c>
       <c r="L139" s="107" t="s">
-        <v>1256</v>
+        <v>1259</v>
       </c>
       <c r="M139" s="107" t="s">
-        <v>1257</v>
+        <v>1260</v>
       </c>
       <c r="N139" s="107"/>
       <c r="O139" s="107"/>
@@ -19944,19 +19942,19 @@
       <c r="G140" s="107"/>
       <c r="H140" s="107"/>
       <c r="I140" s="107" t="s">
-        <v>1258</v>
+        <v>1261</v>
       </c>
       <c r="J140" s="107" t="s">
-        <v>1259</v>
+        <v>1262</v>
       </c>
       <c r="K140" s="107" t="s">
-        <v>1260</v>
+        <v>1263</v>
       </c>
       <c r="L140" s="107" t="s">
-        <v>1261</v>
+        <v>1264</v>
       </c>
       <c r="M140" s="107" t="s">
-        <v>1262</v>
+        <v>1265</v>
       </c>
       <c r="N140" s="107"/>
       <c r="O140" s="107"/>
@@ -19986,19 +19984,19 @@
       <c r="G141" s="107"/>
       <c r="H141" s="107"/>
       <c r="I141" s="107" t="s">
-        <v>1263</v>
+        <v>1266</v>
       </c>
       <c r="J141" s="107" t="s">
-        <v>1264</v>
+        <v>1267</v>
       </c>
       <c r="K141" s="107" t="s">
-        <v>1265</v>
+        <v>1268</v>
       </c>
       <c r="L141" s="107" t="s">
-        <v>1266</v>
+        <v>1269</v>
       </c>
       <c r="M141" s="107" t="s">
-        <v>1267</v>
+        <v>1270</v>
       </c>
       <c r="N141" s="107"/>
       <c r="O141" s="107"/>
@@ -20028,20 +20026,16 @@
       <c r="G142" s="107"/>
       <c r="H142" s="107"/>
       <c r="I142" s="107" t="s">
-        <v>1268</v>
+        <v>1271</v>
       </c>
       <c r="J142" s="107" t="s">
-        <v>1269</v>
+        <v>1272</v>
       </c>
       <c r="K142" s="107" t="s">
-        <v>1270</v>
-      </c>
-      <c r="L142" s="107" t="s">
-        <v>1271</v>
-      </c>
-      <c r="M142" s="107" t="s">
-        <v>1272</v>
-      </c>
+        <v>1273</v>
+      </c>
+      <c r="L142" s="107"/>
+      <c r="M142" s="107"/>
       <c r="N142" s="107"/>
       <c r="O142" s="107"/>
       <c r="P142" s="107"/>
@@ -20070,13 +20064,13 @@
       <c r="G143" s="107"/>
       <c r="H143" s="107"/>
       <c r="I143" s="107" t="s">
-        <v>1273</v>
+        <v>1274</v>
       </c>
       <c r="J143" s="107" t="s">
-        <v>1274</v>
+        <v>1275</v>
       </c>
       <c r="K143" s="107" t="s">
-        <v>1275</v>
+        <v>1276</v>
       </c>
       <c r="L143" s="107"/>
       <c r="M143" s="107"/>
@@ -20108,13 +20102,13 @@
       <c r="G144" s="107"/>
       <c r="H144" s="107"/>
       <c r="I144" s="107" t="s">
-        <v>1276</v>
+        <v>1277</v>
       </c>
       <c r="J144" s="107" t="s">
-        <v>1277</v>
+        <v>1278</v>
       </c>
       <c r="K144" s="107" t="s">
-        <v>1278</v>
+        <v>1279</v>
       </c>
       <c r="L144" s="107"/>
       <c r="M144" s="107"/>
@@ -20146,13 +20140,13 @@
       <c r="G145" s="107"/>
       <c r="H145" s="107"/>
       <c r="I145" s="107" t="s">
-        <v>1279</v>
+        <v>1280</v>
       </c>
       <c r="J145" s="107" t="s">
-        <v>1280</v>
+        <v>1281</v>
       </c>
       <c r="K145" s="107" t="s">
-        <v>1281</v>
+        <v>1282</v>
       </c>
       <c r="L145" s="107"/>
       <c r="M145" s="107"/>
@@ -20184,13 +20178,13 @@
       <c r="G146" s="107"/>
       <c r="H146" s="107"/>
       <c r="I146" s="107" t="s">
-        <v>1282</v>
+        <v>1283</v>
       </c>
       <c r="J146" s="107" t="s">
-        <v>1283</v>
+        <v>1284</v>
       </c>
       <c r="K146" s="107" t="s">
-        <v>1284</v>
+        <v>1285</v>
       </c>
       <c r="L146" s="107"/>
       <c r="M146" s="107"/>
@@ -20219,16 +20213,20 @@
       <c r="D147" s="107"/>
       <c r="E147" s="107"/>
       <c r="F147" s="107"/>
-      <c r="G147" s="107"/>
-      <c r="H147" s="107"/>
+      <c r="G147" s="107" t="s">
+        <v>1286</v>
+      </c>
+      <c r="H147" s="118" t="s">
+        <v>1287</v>
+      </c>
       <c r="I147" s="107" t="s">
-        <v>1285</v>
+        <v>1288</v>
       </c>
       <c r="J147" s="107" t="s">
-        <v>1286</v>
+        <v>1289</v>
       </c>
       <c r="K147" s="107" t="s">
-        <v>1287</v>
+        <v>1290</v>
       </c>
       <c r="L147" s="107"/>
       <c r="M147" s="107"/>
@@ -20257,20 +20255,16 @@
       <c r="D148" s="107"/>
       <c r="E148" s="107"/>
       <c r="F148" s="107"/>
-      <c r="G148" s="107" t="s">
-        <v>1288</v>
-      </c>
-      <c r="H148" s="118" t="s">
-        <v>1289</v>
-      </c>
+      <c r="G148" s="107"/>
+      <c r="H148" s="107"/>
       <c r="I148" s="107" t="s">
-        <v>1290</v>
+        <v>1291</v>
       </c>
       <c r="J148" s="107" t="s">
-        <v>1291</v>
+        <v>1292</v>
       </c>
       <c r="K148" s="107" t="s">
-        <v>1292</v>
+        <v>1293</v>
       </c>
       <c r="L148" s="107"/>
       <c r="M148" s="107"/>
@@ -20302,13 +20296,13 @@
       <c r="G149" s="107"/>
       <c r="H149" s="107"/>
       <c r="I149" s="107" t="s">
-        <v>1293</v>
+        <v>1294</v>
       </c>
       <c r="J149" s="107" t="s">
-        <v>1294</v>
+        <v>1295</v>
       </c>
       <c r="K149" s="107" t="s">
-        <v>1295</v>
+        <v>1296</v>
       </c>
       <c r="L149" s="107"/>
       <c r="M149" s="107"/>
@@ -20340,13 +20334,13 @@
       <c r="G150" s="107"/>
       <c r="H150" s="107"/>
       <c r="I150" s="107" t="s">
-        <v>1296</v>
+        <v>1297</v>
       </c>
       <c r="J150" s="107" t="s">
-        <v>1297</v>
+        <v>1298</v>
       </c>
       <c r="K150" s="107" t="s">
-        <v>1298</v>
+        <v>1299</v>
       </c>
       <c r="L150" s="107"/>
       <c r="M150" s="107"/>
@@ -20375,16 +20369,20 @@
       <c r="D151" s="107"/>
       <c r="E151" s="107"/>
       <c r="F151" s="107"/>
-      <c r="G151" s="107"/>
-      <c r="H151" s="107"/>
+      <c r="G151" s="107" t="s">
+        <v>1300</v>
+      </c>
+      <c r="H151" s="118" t="s">
+        <v>1301</v>
+      </c>
       <c r="I151" s="107" t="s">
-        <v>1299</v>
+        <v>1302</v>
       </c>
       <c r="J151" s="107" t="s">
-        <v>1300</v>
+        <v>1303</v>
       </c>
       <c r="K151" s="107" t="s">
-        <v>1301</v>
+        <v>1304</v>
       </c>
       <c r="L151" s="107"/>
       <c r="M151" s="107"/>
@@ -20413,20 +20411,16 @@
       <c r="D152" s="107"/>
       <c r="E152" s="107"/>
       <c r="F152" s="107"/>
-      <c r="G152" s="107" t="s">
-        <v>1302</v>
-      </c>
-      <c r="H152" s="118" t="s">
-        <v>1303</v>
-      </c>
+      <c r="G152" s="107"/>
+      <c r="H152" s="107"/>
       <c r="I152" s="107" t="s">
-        <v>1304</v>
+        <v>1305</v>
       </c>
       <c r="J152" s="107" t="s">
-        <v>1305</v>
+        <v>1306</v>
       </c>
       <c r="K152" s="107" t="s">
-        <v>1306</v>
+        <v>1307</v>
       </c>
       <c r="L152" s="107"/>
       <c r="M152" s="107"/>
@@ -20458,13 +20452,13 @@
       <c r="G153" s="107"/>
       <c r="H153" s="107"/>
       <c r="I153" s="107" t="s">
-        <v>1307</v>
+        <v>1308</v>
       </c>
       <c r="J153" s="107" t="s">
-        <v>1308</v>
+        <v>1309</v>
       </c>
       <c r="K153" s="107" t="s">
-        <v>1309</v>
+        <v>1310</v>
       </c>
       <c r="L153" s="107"/>
       <c r="M153" s="107"/>
@@ -20496,13 +20490,13 @@
       <c r="G154" s="107"/>
       <c r="H154" s="107"/>
       <c r="I154" s="107" t="s">
-        <v>1310</v>
+        <v>1311</v>
       </c>
       <c r="J154" s="107" t="s">
-        <v>1311</v>
+        <v>1312</v>
       </c>
       <c r="K154" s="107" t="s">
-        <v>1312</v>
+        <v>1313</v>
       </c>
       <c r="L154" s="107"/>
       <c r="M154" s="107"/>
@@ -20534,14 +20528,12 @@
       <c r="G155" s="107"/>
       <c r="H155" s="107"/>
       <c r="I155" s="107" t="s">
-        <v>1313</v>
+        <v>1314</v>
       </c>
       <c r="J155" s="107" t="s">
         <v>1314</v>
       </c>
-      <c r="K155" s="107" t="s">
-        <v>1315</v>
-      </c>
+      <c r="K155" s="107"/>
       <c r="L155" s="107"/>
       <c r="M155" s="107"/>
       <c r="N155" s="107"/>
@@ -20567,17 +20559,27 @@
       <c r="B156" s="107"/>
       <c r="C156" s="107"/>
       <c r="D156" s="107"/>
-      <c r="E156" s="107"/>
-      <c r="F156" s="107"/>
-      <c r="G156" s="107"/>
-      <c r="H156" s="107"/>
+      <c r="E156" s="111" t="s">
+        <v>1315</v>
+      </c>
+      <c r="F156" s="108" t="s">
+        <v>1316</v>
+      </c>
+      <c r="G156" s="107" t="s">
+        <v>1317</v>
+      </c>
+      <c r="H156" s="118" t="s">
+        <v>1318</v>
+      </c>
       <c r="I156" s="107" t="s">
-        <v>1316</v>
+        <v>1319</v>
       </c>
       <c r="J156" s="107" t="s">
-        <v>1316</v>
-      </c>
-      <c r="K156" s="107"/>
+        <v>1319</v>
+      </c>
+      <c r="K156" s="107" t="s">
+        <v>1320</v>
+      </c>
       <c r="L156" s="107"/>
       <c r="M156" s="107"/>
       <c r="N156" s="107"/>
@@ -20603,26 +20605,18 @@
       <c r="B157" s="107"/>
       <c r="C157" s="107"/>
       <c r="D157" s="107"/>
-      <c r="E157" s="111" t="s">
-        <v>1317</v>
-      </c>
-      <c r="F157" s="108" t="s">
-        <v>1318</v>
-      </c>
-      <c r="G157" s="107" t="s">
-        <v>1319</v>
-      </c>
-      <c r="H157" s="118" t="s">
-        <v>1320</v>
-      </c>
+      <c r="E157" s="107"/>
+      <c r="F157" s="107"/>
+      <c r="G157" s="107"/>
+      <c r="H157" s="107"/>
       <c r="I157" s="107" t="s">
         <v>1321</v>
       </c>
       <c r="J157" s="107" t="s">
-        <v>1321</v>
+        <v>1322</v>
       </c>
       <c r="K157" s="107" t="s">
-        <v>1322</v>
+        <v>1323</v>
       </c>
       <c r="L157" s="107"/>
       <c r="M157" s="107"/>
@@ -20654,13 +20648,13 @@
       <c r="G158" s="107"/>
       <c r="H158" s="107"/>
       <c r="I158" s="107" t="s">
-        <v>1323</v>
+        <v>1324</v>
       </c>
       <c r="J158" s="107" t="s">
-        <v>1324</v>
+        <v>1325</v>
       </c>
       <c r="K158" s="107" t="s">
-        <v>1325</v>
+        <v>1326</v>
       </c>
       <c r="L158" s="107"/>
       <c r="M158" s="107"/>
@@ -20692,13 +20686,13 @@
       <c r="G159" s="107"/>
       <c r="H159" s="107"/>
       <c r="I159" s="107" t="s">
-        <v>1326</v>
+        <v>1327</v>
       </c>
       <c r="J159" s="107" t="s">
-        <v>1327</v>
+        <v>1328</v>
       </c>
       <c r="K159" s="107" t="s">
-        <v>1328</v>
+        <v>1329</v>
       </c>
       <c r="L159" s="107"/>
       <c r="M159" s="107"/>
@@ -20730,13 +20724,13 @@
       <c r="G160" s="107"/>
       <c r="H160" s="107"/>
       <c r="I160" s="107" t="s">
-        <v>1329</v>
+        <v>1330</v>
       </c>
       <c r="J160" s="107" t="s">
-        <v>1330</v>
+        <v>1331</v>
       </c>
       <c r="K160" s="107" t="s">
-        <v>1331</v>
+        <v>1332</v>
       </c>
       <c r="L160" s="107"/>
       <c r="M160" s="107"/>
@@ -20765,16 +20759,20 @@
       <c r="D161" s="107"/>
       <c r="E161" s="107"/>
       <c r="F161" s="107"/>
-      <c r="G161" s="107"/>
-      <c r="H161" s="107"/>
+      <c r="G161" s="107" t="s">
+        <v>1333</v>
+      </c>
+      <c r="H161" s="118" t="s">
+        <v>1334</v>
+      </c>
       <c r="I161" s="107" t="s">
-        <v>1332</v>
+        <v>1335</v>
       </c>
       <c r="J161" s="107" t="s">
-        <v>1333</v>
+        <v>1336</v>
       </c>
       <c r="K161" s="107" t="s">
-        <v>1334</v>
+        <v>1337</v>
       </c>
       <c r="L161" s="107"/>
       <c r="M161" s="107"/>
@@ -20803,20 +20801,16 @@
       <c r="D162" s="107"/>
       <c r="E162" s="107"/>
       <c r="F162" s="107"/>
-      <c r="G162" s="107" t="s">
-        <v>1335</v>
-      </c>
-      <c r="H162" s="118" t="s">
-        <v>1336</v>
-      </c>
+      <c r="G162" s="107"/>
+      <c r="H162" s="107"/>
       <c r="I162" s="107" t="s">
-        <v>1337</v>
+        <v>1338</v>
       </c>
       <c r="J162" s="107" t="s">
-        <v>1338</v>
+        <v>1339</v>
       </c>
       <c r="K162" s="107" t="s">
-        <v>1339</v>
+        <v>1340</v>
       </c>
       <c r="L162" s="107"/>
       <c r="M162" s="107"/>
@@ -20848,13 +20842,13 @@
       <c r="G163" s="107"/>
       <c r="H163" s="107"/>
       <c r="I163" s="107" t="s">
-        <v>1340</v>
+        <v>1341</v>
       </c>
       <c r="J163" s="107" t="s">
-        <v>1341</v>
+        <v>1342</v>
       </c>
       <c r="K163" s="107" t="s">
-        <v>1342</v>
+        <v>1343</v>
       </c>
       <c r="L163" s="107"/>
       <c r="M163" s="107"/>
@@ -20886,13 +20880,13 @@
       <c r="G164" s="107"/>
       <c r="H164" s="107"/>
       <c r="I164" s="107" t="s">
-        <v>1343</v>
+        <v>1344</v>
       </c>
       <c r="J164" s="107" t="s">
-        <v>1344</v>
+        <v>1345</v>
       </c>
       <c r="K164" s="107" t="s">
-        <v>1345</v>
+        <v>1346</v>
       </c>
       <c r="L164" s="107"/>
       <c r="M164" s="107"/>
@@ -20924,13 +20918,13 @@
       <c r="G165" s="107"/>
       <c r="H165" s="107"/>
       <c r="I165" s="107" t="s">
-        <v>1346</v>
+        <v>1347</v>
       </c>
       <c r="J165" s="107" t="s">
-        <v>1347</v>
+        <v>1348</v>
       </c>
       <c r="K165" s="107" t="s">
-        <v>1348</v>
+        <v>1349</v>
       </c>
       <c r="L165" s="107"/>
       <c r="M165" s="107"/>
@@ -20959,16 +20953,20 @@
       <c r="D166" s="107"/>
       <c r="E166" s="107"/>
       <c r="F166" s="107"/>
-      <c r="G166" s="107"/>
-      <c r="H166" s="107"/>
+      <c r="G166" s="107" t="s">
+        <v>1350</v>
+      </c>
+      <c r="H166" s="118" t="s">
+        <v>1351</v>
+      </c>
       <c r="I166" s="107" t="s">
-        <v>1349</v>
+        <v>1352</v>
       </c>
       <c r="J166" s="107" t="s">
-        <v>1350</v>
+        <v>1353</v>
       </c>
       <c r="K166" s="107" t="s">
-        <v>1351</v>
+        <v>1354</v>
       </c>
       <c r="L166" s="107"/>
       <c r="M166" s="107"/>
@@ -20997,20 +20995,16 @@
       <c r="D167" s="107"/>
       <c r="E167" s="107"/>
       <c r="F167" s="107"/>
-      <c r="G167" s="107" t="s">
-        <v>1352</v>
-      </c>
-      <c r="H167" s="118" t="s">
-        <v>1353</v>
-      </c>
+      <c r="G167" s="107"/>
+      <c r="H167" s="107"/>
       <c r="I167" s="107" t="s">
-        <v>1354</v>
+        <v>1355</v>
       </c>
       <c r="J167" s="107" t="s">
-        <v>1355</v>
+        <v>1356</v>
       </c>
       <c r="K167" s="107" t="s">
-        <v>1356</v>
+        <v>1357</v>
       </c>
       <c r="L167" s="107"/>
       <c r="M167" s="107"/>
@@ -21042,13 +21036,13 @@
       <c r="G168" s="107"/>
       <c r="H168" s="107"/>
       <c r="I168" s="107" t="s">
-        <v>1357</v>
+        <v>1358</v>
       </c>
       <c r="J168" s="107" t="s">
-        <v>1358</v>
+        <v>1359</v>
       </c>
       <c r="K168" s="107" t="s">
-        <v>1359</v>
+        <v>1360</v>
       </c>
       <c r="L168" s="107"/>
       <c r="M168" s="107"/>
@@ -21080,13 +21074,13 @@
       <c r="G169" s="107"/>
       <c r="H169" s="107"/>
       <c r="I169" s="107" t="s">
-        <v>1360</v>
+        <v>1361</v>
       </c>
       <c r="J169" s="107" t="s">
-        <v>1361</v>
+        <v>1362</v>
       </c>
       <c r="K169" s="107" t="s">
-        <v>1362</v>
+        <v>1363</v>
       </c>
       <c r="L169" s="107"/>
       <c r="M169" s="107"/>
@@ -21115,16 +21109,20 @@
       <c r="D170" s="107"/>
       <c r="E170" s="107"/>
       <c r="F170" s="107"/>
-      <c r="G170" s="107"/>
-      <c r="H170" s="107"/>
+      <c r="G170" s="107" t="s">
+        <v>1364</v>
+      </c>
+      <c r="H170" s="118" t="s">
+        <v>1365</v>
+      </c>
       <c r="I170" s="107" t="s">
-        <v>1363</v>
+        <v>1366</v>
       </c>
       <c r="J170" s="107" t="s">
-        <v>1364</v>
+        <v>1367</v>
       </c>
       <c r="K170" s="107" t="s">
-        <v>1365</v>
+        <v>1368</v>
       </c>
       <c r="L170" s="107"/>
       <c r="M170" s="107"/>
@@ -21153,22 +21151,20 @@
       <c r="D171" s="107"/>
       <c r="E171" s="107"/>
       <c r="F171" s="107"/>
-      <c r="G171" s="107" t="s">
-        <v>1366</v>
-      </c>
-      <c r="H171" s="118" t="s">
-        <v>1367</v>
-      </c>
+      <c r="G171" s="107"/>
+      <c r="H171" s="107"/>
       <c r="I171" s="107" t="s">
-        <v>1368</v>
+        <v>1369</v>
       </c>
       <c r="J171" s="107" t="s">
-        <v>1369</v>
+        <v>1370</v>
       </c>
       <c r="K171" s="107" t="s">
-        <v>1370</v>
-      </c>
-      <c r="L171" s="107"/>
+        <v>1371</v>
+      </c>
+      <c r="L171" s="107" t="s">
+        <v>1372</v>
+      </c>
       <c r="M171" s="107"/>
       <c r="N171" s="107"/>
       <c r="O171" s="107"/>
@@ -21198,17 +21194,15 @@
       <c r="G172" s="107"/>
       <c r="H172" s="107"/>
       <c r="I172" s="107" t="s">
-        <v>1371</v>
+        <v>1373</v>
       </c>
       <c r="J172" s="107" t="s">
-        <v>1372</v>
+        <v>1374</v>
       </c>
       <c r="K172" s="107" t="s">
-        <v>1373</v>
-      </c>
-      <c r="L172" s="107" t="s">
-        <v>1374</v>
-      </c>
+        <v>1375</v>
+      </c>
+      <c r="L172" s="107"/>
       <c r="M172" s="107"/>
       <c r="N172" s="107"/>
       <c r="O172" s="107"/>
@@ -21235,16 +21229,20 @@
       <c r="D173" s="107"/>
       <c r="E173" s="107"/>
       <c r="F173" s="107"/>
-      <c r="G173" s="107"/>
-      <c r="H173" s="107"/>
+      <c r="G173" s="107" t="s">
+        <v>1376</v>
+      </c>
+      <c r="H173" s="118" t="s">
+        <v>1377</v>
+      </c>
       <c r="I173" s="107" t="s">
-        <v>1375</v>
+        <v>1378</v>
       </c>
       <c r="J173" s="107" t="s">
-        <v>1376</v>
+        <v>1379</v>
       </c>
       <c r="K173" s="107" t="s">
-        <v>1377</v>
+        <v>1380</v>
       </c>
       <c r="L173" s="107"/>
       <c r="M173" s="107"/>
@@ -21273,20 +21271,16 @@
       <c r="D174" s="107"/>
       <c r="E174" s="107"/>
       <c r="F174" s="107"/>
-      <c r="G174" s="107" t="s">
-        <v>1378</v>
-      </c>
-      <c r="H174" s="118" t="s">
-        <v>1379</v>
-      </c>
+      <c r="G174" s="107"/>
+      <c r="H174" s="107"/>
       <c r="I174" s="107" t="s">
-        <v>1380</v>
+        <v>1381</v>
       </c>
       <c r="J174" s="107" t="s">
-        <v>1381</v>
+        <v>1382</v>
       </c>
       <c r="K174" s="107" t="s">
-        <v>1382</v>
+        <v>1383</v>
       </c>
       <c r="L174" s="107"/>
       <c r="M174" s="107"/>
@@ -21318,13 +21312,13 @@
       <c r="G175" s="107"/>
       <c r="H175" s="107"/>
       <c r="I175" s="107" t="s">
-        <v>1383</v>
+        <v>1384</v>
       </c>
       <c r="J175" s="107" t="s">
-        <v>1384</v>
+        <v>1385</v>
       </c>
       <c r="K175" s="107" t="s">
-        <v>1385</v>
+        <v>1386</v>
       </c>
       <c r="L175" s="107"/>
       <c r="M175" s="107"/>
@@ -21356,13 +21350,13 @@
       <c r="G176" s="107"/>
       <c r="H176" s="107"/>
       <c r="I176" s="107" t="s">
-        <v>1386</v>
+        <v>1387</v>
       </c>
       <c r="J176" s="107" t="s">
-        <v>1387</v>
+        <v>1388</v>
       </c>
       <c r="K176" s="107" t="s">
-        <v>1388</v>
+        <v>1389</v>
       </c>
       <c r="L176" s="107"/>
       <c r="M176" s="107"/>
@@ -21391,16 +21385,20 @@
       <c r="D177" s="107"/>
       <c r="E177" s="107"/>
       <c r="F177" s="107"/>
-      <c r="G177" s="107"/>
-      <c r="H177" s="107"/>
+      <c r="G177" s="107" t="s">
+        <v>1390</v>
+      </c>
+      <c r="H177" s="119" t="s">
+        <v>1391</v>
+      </c>
       <c r="I177" s="107" t="s">
-        <v>1389</v>
+        <v>1392</v>
       </c>
       <c r="J177" s="107" t="s">
-        <v>1390</v>
+        <v>1393</v>
       </c>
       <c r="K177" s="107" t="s">
-        <v>1391</v>
+        <v>1394</v>
       </c>
       <c r="L177" s="107"/>
       <c r="M177" s="107"/>
@@ -21429,23 +21427,23 @@
       <c r="D178" s="107"/>
       <c r="E178" s="107"/>
       <c r="F178" s="107"/>
-      <c r="G178" s="107" t="s">
-        <v>1392</v>
-      </c>
-      <c r="H178" s="119" t="s">
-        <v>1393</v>
-      </c>
+      <c r="G178" s="107"/>
+      <c r="H178" s="107"/>
       <c r="I178" s="107" t="s">
-        <v>1394</v>
+        <v>1395</v>
       </c>
       <c r="J178" s="107" t="s">
-        <v>1395</v>
+        <v>1396</v>
       </c>
       <c r="K178" s="107" t="s">
-        <v>1396</v>
-      </c>
-      <c r="L178" s="107"/>
-      <c r="M178" s="107"/>
+        <v>1397</v>
+      </c>
+      <c r="L178" s="107" t="s">
+        <v>1398</v>
+      </c>
+      <c r="M178" s="107" t="s">
+        <v>1399</v>
+      </c>
       <c r="N178" s="107"/>
       <c r="O178" s="107"/>
       <c r="P178" s="107"/>
@@ -21474,19 +21472,19 @@
       <c r="G179" s="107"/>
       <c r="H179" s="107"/>
       <c r="I179" s="107" t="s">
-        <v>1397</v>
+        <v>1400</v>
       </c>
       <c r="J179" s="107" t="s">
-        <v>1398</v>
+        <v>1401</v>
       </c>
       <c r="K179" s="107" t="s">
-        <v>1399</v>
+        <v>1402</v>
       </c>
       <c r="L179" s="107" t="s">
-        <v>1400</v>
+        <v>1403</v>
       </c>
       <c r="M179" s="107" t="s">
-        <v>1401</v>
+        <v>1404</v>
       </c>
       <c r="N179" s="107"/>
       <c r="O179" s="107"/>
@@ -21506,48 +21504,7 @@
       <c r="AC179" s="107"/>
       <c r="AD179" s="107"/>
     </row>
-    <row r="180" customFormat="false" ht="9.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A180" s="107"/>
-      <c r="B180" s="107"/>
-      <c r="C180" s="107"/>
-      <c r="D180" s="107"/>
-      <c r="E180" s="107"/>
-      <c r="F180" s="107"/>
-      <c r="G180" s="107"/>
-      <c r="H180" s="107"/>
-      <c r="I180" s="107" t="s">
-        <v>1402</v>
-      </c>
-      <c r="J180" s="107" t="s">
-        <v>1403</v>
-      </c>
-      <c r="K180" s="107" t="s">
-        <v>1404</v>
-      </c>
-      <c r="L180" s="107" t="s">
-        <v>1405</v>
-      </c>
-      <c r="M180" s="107" t="s">
-        <v>1406</v>
-      </c>
-      <c r="N180" s="107"/>
-      <c r="O180" s="107"/>
-      <c r="P180" s="107"/>
-      <c r="Q180" s="107"/>
-      <c r="R180" s="107"/>
-      <c r="S180" s="107"/>
-      <c r="T180" s="107"/>
-      <c r="U180" s="107"/>
-      <c r="V180" s="107"/>
-      <c r="W180" s="107"/>
-      <c r="X180" s="107"/>
-      <c r="Y180" s="107"/>
-      <c r="Z180" s="107"/>
-      <c r="AA180" s="107"/>
-      <c r="AB180" s="107"/>
-      <c r="AC180" s="107"/>
-      <c r="AD180" s="107"/>
-    </row>
+    <row r="1047820" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1047821" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1047822" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1047823" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -22305,7 +22262,7 @@
     <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
-  <autoFilter ref="A1:Y180"/>
+  <autoFilter ref="A1:Y179"/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>

</xml_diff>

<commit_message>
Dev #384 adjust specs after change
</commit_message>
<xml_diff>
--- a/spec/fixtures/files/reduced_categories_table.xlsx
+++ b/spec/fixtures/files/reduced_categories_table.xlsx
@@ -8,14 +8,14 @@
     <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
   </bookViews>
   <sheets>
-    <sheet name="Demographics" sheetId="1" state="visible" r:id="rId2"/>
-    <sheet name="CIN-CLA" sheetId="2" state="visible" r:id="rId3"/>
-    <sheet name="Absence-Exclusion" sheetId="3" state="visible" r:id="rId4"/>
-    <sheet name="Attainment" sheetId="4" state="visible" r:id="rId5"/>
+    <sheet name="IA_Demographics" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="IA_CIN-CLA" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="IA_Absence-Exclusion" sheetId="3" state="visible" r:id="rId4"/>
+    <sheet name="IA_Attainment" sheetId="4" state="visible" r:id="rId5"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="true" localSheetId="3" name="_xlnm._FilterDatabase" vbProcedure="false">Attainment!$A$1:$Y$179</definedName>
-    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Demographics!$A$5:$AM$40</definedName>
+    <definedName function="false" hidden="true" localSheetId="3" name="_xlnm._FilterDatabase" vbProcedure="false">IA_Attainment!$A$1:$Y$179</definedName>
+    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">IA_Demographics!$A$5:$AM$40</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -5207,9 +5207,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>27000</xdr:colOff>
+      <xdr:colOff>26640</xdr:colOff>
       <xdr:row>44</xdr:row>
-      <xdr:rowOff>132120</xdr:rowOff>
+      <xdr:rowOff>131760</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -5223,7 +5223,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="22943160" y="8239320"/>
-          <a:ext cx="27000" cy="7920"/>
+          <a:ext cx="26640" cy="7560"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>

</xml_diff>

<commit_message>
Dev #453 remove sub from subcategories
</commit_message>
<xml_diff>
--- a/spec/fixtures/files/reduced_categories_table.xlsx
+++ b/spec/fixtures/files/reduced_categories_table.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="IA_Demographics" sheetId="1" state="visible" r:id="rId2"/>
@@ -89,13 +89,13 @@
     <t xml:space="preserve">Category (L1) Description</t>
   </si>
   <si>
-    <t xml:space="preserve">Sub-category (L2)</t>
+    <t xml:space="preserve">Category (L2)</t>
   </si>
   <si>
     <t xml:space="preserve">Category (L2) Description</t>
   </si>
   <si>
-    <t xml:space="preserve">Sub-category (L3)</t>
+    <t xml:space="preserve">Category (L3)</t>
   </si>
   <si>
     <t xml:space="preserve">Category (L3) Description</t>
@@ -5207,9 +5207,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>26640</xdr:colOff>
+      <xdr:colOff>25920</xdr:colOff>
       <xdr:row>44</xdr:row>
-      <xdr:rowOff>131760</xdr:rowOff>
+      <xdr:rowOff>131040</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -5223,7 +5223,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="22943160" y="8239320"/>
-          <a:ext cx="26640" cy="7560"/>
+          <a:ext cx="25920" cy="6840"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -5249,10 +5249,10 @@
   </sheetPr>
   <dimension ref="A1:AM1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="55" zoomScaleNormal="55" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="55" zoomScaleNormal="55" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="5" topLeftCell="A35" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="I48" activeCellId="0" sqref="I48"/>
+      <selection pane="bottomLeft" activeCell="I5" activeCellId="0" sqref="I5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -9222,7 +9222,7 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="55" zoomScaleNormal="55" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="5" topLeftCell="A52" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="I6" activeCellId="0" sqref="I6"/>
+      <selection pane="bottomLeft" activeCell="I5" activeCellId="0" sqref="I5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -11376,8 +11376,8 @@
   </sheetPr>
   <dimension ref="A1:AD1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A13" colorId="64" zoomScale="55" zoomScaleNormal="55" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I50" activeCellId="0" sqref="I50"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="55" zoomScaleNormal="55" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H5" activeCellId="0" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -14415,10 +14415,10 @@
   </sheetPr>
   <dimension ref="A1:AD1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="55" zoomScaleNormal="55" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="55" zoomScaleNormal="55" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="A50" activeCellId="0" sqref="A50"/>
+      <selection pane="bottomLeft" activeCell="H1" activeCellId="0" sqref="H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>